<commit_message>
Selenium grid 4 compatible
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Book1.xlsx
+++ b/src/test/resources/excel/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bomaseko\eclipse-workspace\MultiplyAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D5F217-E7E8-4BB5-B3E9-A8D4EDDADDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344DC249-0E78-4819-A203-BD0FA23A0D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{290FA3F8-6C32-43F1-8ED4-F2A44DB688D9}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{290FA3F8-6C32-43F1-8ED4-F2A44DB688D9}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>testname</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>QEtCVG9remFuMjAyMQ==</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -508,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E20413-DA9E-4BED-8FCD-A1CA282FA624}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +615,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FA2802-445E-49FF-8269-F5C3316F0F48}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +672,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -800,6 +803,29 @@
       </c>
       <c r="G7" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the surefire plugin for pom execution
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Book1.xlsx
+++ b/src/test/resources/excel/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bomaseko\eclipse-workspace\MultiplyAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344DC249-0E78-4819-A203-BD0FA23A0D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44F26D6-3707-40B3-8F4F-26197745BF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{290FA3F8-6C32-43F1-8ED4-F2A44DB688D9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{290FA3F8-6C32-43F1-8ED4-F2A44DB688D9}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E20413-DA9E-4BED-8FCD-A1CA282FA624}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FA2802-445E-49FF-8269-F5C3316F0F48}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Admin UI TC implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Book1.xlsx
+++ b/src/test/resources/excel/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bomaseko\eclipse-workspace\MultiplyAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44F26D6-3707-40B3-8F4F-26197745BF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045AFF0D-C3A8-492B-9FA4-AE44E112C84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{290FA3F8-6C32-43F1-8ED4-F2A44DB688D9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>testname</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>campaignManagementTest</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>To check if the user is able to create a campaign</t>
   </si>
 </sst>
 </file>
@@ -509,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E20413-DA9E-4BED-8FCD-A1CA282FA624}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -621,6 +630,23 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -631,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FA2802-445E-49FF-8269-F5C3316F0F48}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,7 +698,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -741,7 +767,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -810,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -826,6 +852,29 @@
       </c>
       <c r="G8" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>